<commit_message>
Update with data Chris sent on 5/4/2020
</commit_message>
<xml_diff>
--- a/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
+++ b/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6323" yWindow="3810" windowWidth="12878" windowHeight="3413" activeTab="1"/>
+    <workbookView xWindow="5093" yWindow="1253" windowWidth="12878" windowHeight="3413" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="205">
   <si>
     <t>BRPSPTY BAU Renewable Portfolio Std Percentage This Year</t>
   </si>
@@ -695,23 +695,21 @@
     <t>Need MWh factoring in approximate curtailment</t>
   </si>
   <si>
-    <t xml:space="preserve">increase slightly because results coming in below </t>
-  </si>
-  <si>
-    <t>round up</t>
+    <t>adjustment found after observing endogenous curtailment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="0.000000000000000%"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="34" x14ac:knownFonts="1">
     <font>
@@ -1358,7 +1356,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1461,7 +1459,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1471,7 +1471,7 @@
     <xf numFmtId="0" fontId="23" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -2344,66 +2344,66 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B10" s="17" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B11" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B20" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B22" s="4" t="s">
         <v>87</v>
       </c>
@@ -2723,7 +2723,7 @@
     <row r="7" spans="1:3" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:3" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:3" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:3" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="17" t="str">
         <f>'EIA-CHP Table 10'!A23</f>
         <v>Total electric industry retail sales</v>
@@ -2733,7 +2733,7 @@
         <v>257267937</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="17" t="s">
         <v>164</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="17" t="str">
         <f>'EIA-CHP Table 10'!A27</f>
         <v>Unaccounted</v>
@@ -2755,7 +2755,7 @@
         <v>1711477</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="17" t="s">
         <v>165</v>
       </c>
@@ -2764,8 +2764,8 @@
         <v>18093849</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:3" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="17" t="s">
         <v>148</v>
       </c>
@@ -2774,8 +2774,8 @@
         <v>0.9342906317436509</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:15" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="17" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="str">
         <f>'CHP notes from the IRP'!K4</f>
         <v>% decline</v>
@@ -2785,7 +2785,7 @@
         <v>0.83543286649820914</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="17" t="s">
         <v>166</v>
       </c>
@@ -2794,8 +2794,8 @@
         <v>0.16456713350179086</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:15" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B20" s="17">
         <v>2017</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B21" s="37">
         <v>1</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>0.16456713350179086</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="17" customFormat="1" ht="14.55" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="23" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="25" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
@@ -3060,8 +3060,8 @@
   </sheetPr>
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3232,9 +3232,9 @@
         <f>'SB100 RPS and sales adjustment'!N34</f>
         <v>0.44028661207461534</v>
       </c>
-      <c r="O2" s="5">
-        <f>'SB100 RPS and sales adjustment'!$O$36</f>
-        <v>0.46750000000000003</v>
+      <c r="O2" s="53">
+        <f>'SB100 RPS and sales adjustment'!$O$34</f>
+        <v>0.46573331721057465</v>
       </c>
       <c r="P2" s="5">
         <v>0</v>
@@ -3285,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="AF2" s="5">
-        <f t="shared" ref="Q2:AI2" si="0">AE2</f>
+        <f t="shared" ref="AF2:AI2" si="0">AE2</f>
         <v>0</v>
       </c>
       <c r="AG2" s="5">
@@ -3309,10 +3309,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ43"/>
+  <dimension ref="A1:AJ40"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4530,7 +4530,7 @@
         <v>302979642.44538897</v>
       </c>
     </row>
-    <row r="25" spans="1:36" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B25" s="45"/>
       <c r="C25" s="45"/>
       <c r="D25" s="45"/>
@@ -4566,13 +4566,13 @@
       <c r="AH25" s="46"/>
       <c r="AI25" s="46"/>
     </row>
-    <row r="26" spans="1:36" s="43" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:36" s="43" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="43" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="1:36" s="51" customFormat="1" ht="14.55" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:36" s="51" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:36" s="51" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="1:36" s="51" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
         <v>190</v>
       </c>
@@ -4713,8 +4713,8 @@
         <v>29274400</v>
       </c>
     </row>
-    <row r="29" spans="1:36" s="51" customFormat="1" ht="14.55" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:36" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:36" s="51" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A30" s="8" t="s">
         <v>188</v>
       </c>
@@ -4796,7 +4796,7 @@
       <c r="AI30" s="19"/>
       <c r="AJ30" s="19"/>
     </row>
-    <row r="31" spans="1:36" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
         <v>202</v>
       </c>
@@ -4867,7 +4867,7 @@
       <c r="AI31" s="19"/>
       <c r="AJ31" s="19"/>
     </row>
-    <row r="32" spans="1:36" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
         <v>203</v>
       </c>
@@ -4949,7 +4949,7 @@
       <c r="AI32" s="19"/>
       <c r="AJ32" s="19"/>
     </row>
-    <row r="33" spans="1:36" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.45">
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
@@ -4961,8 +4961,7 @@
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
+      <c r="O33" s="54"/>
       <c r="Q33" s="19"/>
       <c r="R33" s="19"/>
       <c r="S33" s="19"/>
@@ -4984,7 +4983,7 @@
       <c r="AI33" s="19"/>
       <c r="AJ33" s="19"/>
     </row>
-    <row r="34" spans="1:36" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A34" s="8" t="s">
         <v>194</v>
       </c>
@@ -5040,11 +5039,13 @@
         <f t="shared" si="12"/>
         <v>0.44028661207461534</v>
       </c>
-      <c r="O34" s="56">
+      <c r="O34" s="58">
         <f t="shared" si="12"/>
         <v>0.46573331721057465</v>
       </c>
-      <c r="P34" s="45"/>
+      <c r="P34" s="19" t="s">
+        <v>204</v>
+      </c>
       <c r="Q34" s="45"/>
       <c r="R34" s="45"/>
       <c r="S34" s="45"/>
@@ -5065,22 +5066,19 @@
       <c r="AH34" s="45"/>
       <c r="AI34" s="45"/>
     </row>
-    <row r="35" spans="1:36" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B35" s="52"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="52" t="s">
-        <v>204</v>
-      </c>
-      <c r="N35" s="52"/>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
+      <c r="N35" s="45"/>
       <c r="O35" s="52"/>
       <c r="P35" s="45"/>
       <c r="Q35" s="45"/>
@@ -5103,7 +5101,7 @@
       <c r="AH35" s="45"/>
       <c r="AI35" s="45"/>
     </row>
-    <row r="36" spans="1:36" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.45">
       <c r="B36" s="49"/>
       <c r="C36" s="49"/>
       <c r="D36" s="49"/>
@@ -5115,382 +5113,330 @@
       <c r="J36" s="49"/>
       <c r="K36" s="49"/>
       <c r="L36" s="49"/>
-      <c r="M36" s="49" t="s">
-        <v>205</v>
-      </c>
+      <c r="M36" s="49"/>
       <c r="N36" s="49"/>
-      <c r="O36" s="50">
-        <v>0.46750000000000003</v>
-      </c>
-    </row>
-    <row r="37" spans="1:36" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B37" s="49"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="49"/>
-      <c r="O37" s="49"/>
-    </row>
-    <row r="38" spans="1:36" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="49"/>
-      <c r="I38" s="49"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="49"/>
-    </row>
-    <row r="39" spans="1:36" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="49"/>
-      <c r="O39" s="49"/>
-    </row>
-    <row r="40" spans="1:36" s="43" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="A40" s="43" t="s">
+      <c r="O36" s="49"/>
+    </row>
+    <row r="37" spans="1:36" s="43" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="48">
+      <c r="B37" s="48">
         <v>2017</v>
       </c>
-      <c r="C40" s="48">
+      <c r="C37" s="48">
         <v>2018</v>
       </c>
-      <c r="D40" s="48">
+      <c r="D37" s="48">
         <v>2019</v>
       </c>
-      <c r="E40" s="48">
+      <c r="E37" s="48">
         <v>2020</v>
       </c>
-      <c r="F40" s="48">
+      <c r="F37" s="48">
         <v>2021</v>
       </c>
-      <c r="G40" s="48">
+      <c r="G37" s="48">
         <v>2022</v>
       </c>
-      <c r="H40" s="48">
+      <c r="H37" s="48">
         <v>2023</v>
       </c>
-      <c r="I40" s="48">
+      <c r="I37" s="48">
         <v>2024</v>
       </c>
-      <c r="J40" s="48">
+      <c r="J37" s="48">
         <v>2025</v>
       </c>
-      <c r="K40" s="48">
+      <c r="K37" s="48">
         <v>2026</v>
       </c>
-      <c r="L40" s="48">
+      <c r="L37" s="48">
         <v>2027</v>
       </c>
-      <c r="M40" s="48">
+      <c r="M37" s="48">
         <v>2028</v>
       </c>
-      <c r="N40" s="48">
+      <c r="N37" s="48">
         <v>2029</v>
       </c>
-      <c r="O40" s="48">
+      <c r="O37" s="48">
         <v>2030</v>
       </c>
-      <c r="P40" s="48">
+      <c r="P37" s="48">
         <v>2031</v>
       </c>
-      <c r="Q40" s="48">
+      <c r="Q37" s="48">
         <v>2032</v>
       </c>
-      <c r="R40" s="48">
+      <c r="R37" s="48">
         <v>2033</v>
       </c>
-      <c r="S40" s="48">
+      <c r="S37" s="48">
         <v>2034</v>
       </c>
-      <c r="T40" s="48">
+      <c r="T37" s="48">
         <v>2035</v>
       </c>
-      <c r="U40" s="48">
+      <c r="U37" s="48">
         <v>2036</v>
       </c>
-      <c r="V40" s="48">
+      <c r="V37" s="48">
         <v>2037</v>
       </c>
-      <c r="W40" s="48">
+      <c r="W37" s="48">
         <v>2038</v>
       </c>
-      <c r="X40" s="48">
+      <c r="X37" s="48">
         <v>2039</v>
       </c>
-      <c r="Y40" s="48">
+      <c r="Y37" s="48">
         <v>2040</v>
       </c>
-      <c r="Z40" s="48">
+      <c r="Z37" s="48">
         <v>2041</v>
       </c>
-      <c r="AA40" s="48">
+      <c r="AA37" s="48">
         <v>2042</v>
       </c>
-      <c r="AB40" s="48">
+      <c r="AB37" s="48">
         <v>2043</v>
       </c>
-      <c r="AC40" s="48">
+      <c r="AC37" s="48">
         <v>2044</v>
       </c>
-      <c r="AD40" s="48">
+      <c r="AD37" s="48">
         <v>2045</v>
       </c>
-      <c r="AE40" s="48">
+      <c r="AE37" s="48">
         <v>2046</v>
       </c>
-      <c r="AF40" s="48">
+      <c r="AF37" s="48">
         <v>2047</v>
       </c>
-      <c r="AG40" s="48">
+      <c r="AG37" s="48">
         <v>2048</v>
       </c>
-      <c r="AH40" s="48">
+      <c r="AH37" s="48">
         <v>2049</v>
       </c>
-      <c r="AI40" s="48">
+      <c r="AI37" s="48">
         <v>2050</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="A41" s="8" t="s">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A38" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="O41" s="8">
+      <c r="O38" s="8">
         <v>0.6</v>
       </c>
-      <c r="P41" s="8">
-        <f>O41+($AD$41-$O$41)/15</f>
+      <c r="P38" s="8">
+        <f>O38+($AD$38-$O$38)/15</f>
         <v>0.62666666666666659</v>
       </c>
-      <c r="Q41" s="8">
-        <f t="shared" ref="Q41:AC41" si="13">P41+($AD$41-$O$41)/15</f>
+      <c r="Q38" s="8">
+        <f t="shared" ref="Q38:AC38" si="13">P38+($AD$38-$O$38)/15</f>
         <v>0.65333333333333321</v>
       </c>
-      <c r="R41" s="8">
+      <c r="R38" s="8">
         <f t="shared" si="13"/>
         <v>0.67999999999999983</v>
       </c>
-      <c r="S41" s="8">
+      <c r="S38" s="8">
         <f t="shared" si="13"/>
         <v>0.70666666666666644</v>
       </c>
-      <c r="T41" s="8">
+      <c r="T38" s="8">
         <f t="shared" si="13"/>
         <v>0.73333333333333306</v>
       </c>
-      <c r="U41" s="8">
+      <c r="U38" s="8">
         <f t="shared" si="13"/>
         <v>0.75999999999999968</v>
       </c>
-      <c r="V41" s="8">
+      <c r="V38" s="8">
         <f t="shared" si="13"/>
         <v>0.78666666666666629</v>
       </c>
-      <c r="W41" s="8">
+      <c r="W38" s="8">
         <f t="shared" si="13"/>
         <v>0.81333333333333291</v>
       </c>
-      <c r="X41" s="8">
+      <c r="X38" s="8">
         <f t="shared" si="13"/>
         <v>0.83999999999999952</v>
       </c>
-      <c r="Y41" s="8">
+      <c r="Y38" s="8">
         <f t="shared" si="13"/>
         <v>0.86666666666666614</v>
       </c>
-      <c r="Z41" s="8">
+      <c r="Z38" s="8">
         <f t="shared" si="13"/>
         <v>0.89333333333333276</v>
       </c>
-      <c r="AA41" s="8">
+      <c r="AA38" s="8">
         <f t="shared" si="13"/>
         <v>0.91999999999999937</v>
       </c>
-      <c r="AB41" s="8">
+      <c r="AB38" s="8">
         <f t="shared" si="13"/>
         <v>0.94666666666666599</v>
       </c>
-      <c r="AC41" s="8">
+      <c r="AC38" s="8">
         <f t="shared" si="13"/>
         <v>0.97333333333333261</v>
       </c>
-      <c r="AD41" s="8">
+      <c r="AD38" s="8">
         <v>1</v>
       </c>
-      <c r="AE41" s="8">
+      <c r="AE38" s="8">
         <v>1</v>
       </c>
-      <c r="AF41" s="8">
+      <c r="AF38" s="8">
         <v>1</v>
       </c>
-      <c r="AG41" s="8">
+      <c r="AG38" s="8">
         <v>1</v>
       </c>
-      <c r="AH41" s="8">
+      <c r="AH38" s="8">
         <v>1</v>
       </c>
-      <c r="AI41" s="8">
+      <c r="AI38" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="A42" s="8" t="s">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="A39" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="P42" s="8">
-        <f>P41-O41</f>
+      <c r="P39" s="8">
+        <f>P38-O38</f>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="Q42" s="8">
-        <f t="shared" ref="Q42:AD42" si="14">Q41-P41</f>
+      <c r="Q39" s="8">
+        <f t="shared" ref="Q39:AD39" si="14">Q38-P38</f>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="R42" s="8">
+      <c r="R39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="S42" s="8">
+      <c r="S39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="T42" s="8">
+      <c r="T39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="U42" s="8">
+      <c r="U39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="V42" s="8">
+      <c r="V39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="W42" s="8">
+      <c r="W39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="X42" s="8">
+      <c r="X39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="Y42" s="8">
+      <c r="Y39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="Z42" s="8">
+      <c r="Z39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="AA42" s="8">
+      <c r="AA39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="AB42" s="8">
+      <c r="AB39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="AC42" s="8">
+      <c r="AC39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666666616E-2</v>
       </c>
-      <c r="AD42" s="8">
+      <c r="AD39" s="8">
         <f t="shared" si="14"/>
         <v>2.6666666666667393E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="O43" s="50">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.45">
+      <c r="O40" s="50">
         <f>O34</f>
         <v>0.46573331721057465</v>
       </c>
-      <c r="P43" s="50">
-        <f>O43+P42</f>
+      <c r="P40" s="50">
+        <f>O40+P39</f>
         <v>0.49239998387724127</v>
       </c>
-      <c r="Q43" s="50">
-        <f t="shared" ref="Q43:AD43" si="15">P43+Q42</f>
+      <c r="Q40" s="50">
+        <f t="shared" ref="Q40:AD40" si="15">P40+Q39</f>
         <v>0.51906665054390788</v>
       </c>
-      <c r="R43" s="50">
+      <c r="R40" s="50">
         <f t="shared" si="15"/>
         <v>0.5457333172105745</v>
       </c>
-      <c r="S43" s="50">
+      <c r="S40" s="50">
         <f t="shared" si="15"/>
         <v>0.57239998387724111</v>
       </c>
-      <c r="T43" s="50">
+      <c r="T40" s="50">
         <f t="shared" si="15"/>
         <v>0.59906665054390773</v>
       </c>
-      <c r="U43" s="50">
+      <c r="U40" s="50">
         <f t="shared" si="15"/>
         <v>0.62573331721057435</v>
       </c>
-      <c r="V43" s="50">
+      <c r="V40" s="50">
         <f t="shared" si="15"/>
         <v>0.65239998387724096</v>
       </c>
-      <c r="W43" s="50">
+      <c r="W40" s="50">
         <f t="shared" si="15"/>
         <v>0.67906665054390758</v>
       </c>
-      <c r="X43" s="50">
+      <c r="X40" s="50">
         <f t="shared" si="15"/>
         <v>0.7057333172105742</v>
       </c>
-      <c r="Y43" s="50">
+      <c r="Y40" s="50">
         <f t="shared" si="15"/>
         <v>0.73239998387724081</v>
       </c>
-      <c r="Z43" s="50">
+      <c r="Z40" s="50">
         <f t="shared" si="15"/>
         <v>0.75906665054390743</v>
       </c>
-      <c r="AA43" s="50">
+      <c r="AA40" s="50">
         <f t="shared" si="15"/>
         <v>0.78573331721057404</v>
       </c>
-      <c r="AB43" s="50">
+      <c r="AB40" s="50">
         <f t="shared" si="15"/>
         <v>0.81239998387724066</v>
       </c>
-      <c r="AC43" s="50">
+      <c r="AC40" s="50">
         <f t="shared" si="15"/>
         <v>0.83906665054390728</v>
       </c>
-      <c r="AD43" s="50">
+      <c r="AD40" s="50">
         <f t="shared" si="15"/>
         <v>0.86573331721057467</v>
       </c>
-      <c r="AE43" s="8">
+      <c r="AE40" s="8">
         <v>1</v>
       </c>
     </row>
@@ -6569,7 +6515,7 @@
         <v>5268000</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -6676,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -6783,7 +6729,7 @@
         <v>900000</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -6890,7 +6836,7 @@
         <v>1053400</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -6997,7 +6943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -7104,7 +7050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -7211,7 +7157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -7318,7 +7264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:35" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -7459,17 +7405,17 @@
         <v>25854400</v>
       </c>
     </row>
-    <row r="29" spans="1:35" s="13" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:35" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>3420000</v>
       </c>
@@ -8614,23 +8560,23 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="23.55" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A50" s="38"/>
     </row>
-    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A51" s="40">
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="41" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="42"/>
     </row>
-    <row r="54" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="42"/>
     </row>
   </sheetData>
@@ -8657,103 +8603,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
     </row>
     <row r="2" spans="1:29" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="55"/>
     </row>
     <row r="3" spans="1:29" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="54"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="56"/>
+      <c r="AB3" s="56"/>
+      <c r="AC3" s="56"/>
     </row>
     <row r="4" spans="1:29" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
@@ -10535,7 +10481,7 @@
         <v>211092922</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A24" s="20" t="s">
         <v>138</v>
       </c>
@@ -10624,7 +10570,7 @@
         <v>9653985</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A25" s="20" t="s">
         <v>139</v>
       </c>
@@ -10713,7 +10659,7 @@
         <v>523792</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A26" s="20" t="s">
         <v>140</v>
       </c>
@@ -10802,7 +10748,7 @@
         <v>16026342</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A27" s="20" t="s">
         <v>141</v>
       </c>
@@ -10891,7 +10837,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A28" s="20" t="s">
         <v>143</v>
       </c>
@@ -10980,7 +10926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A29" s="29" t="s">
         <v>144</v>
       </c>
@@ -11069,7 +11015,7 @@
         <v>237014131</v>
       </c>
     </row>
-    <row r="30" spans="1:29" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A30" s="20" t="s">
         <v>145</v>
       </c>
@@ -11158,7 +11104,7 @@
         <v>-66087034</v>
       </c>
     </row>
-    <row r="31" spans="1:29" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A31" s="22" t="s">
         <v>146</v>
       </c>
@@ -11247,40 +11193,40 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="55" t="s">
+    <row r="32" spans="1:29" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="55"/>
-      <c r="M32" s="55"/>
-      <c r="N32" s="55"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="55"/>
-      <c r="Q32" s="55"/>
-      <c r="R32" s="55"/>
-      <c r="S32" s="55"/>
-      <c r="T32" s="55"/>
-      <c r="U32" s="55"/>
-      <c r="V32" s="55"/>
-      <c r="W32" s="55"/>
-      <c r="X32" s="55"/>
-      <c r="Y32" s="55"/>
-      <c r="Z32" s="55"/>
-      <c r="AA32" s="55"/>
-      <c r="AB32" s="55"/>
-      <c r="AC32" s="55"/>
-    </row>
-    <row r="33" spans="1:29" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="57"/>
+      <c r="L32" s="57"/>
+      <c r="M32" s="57"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="57"/>
+      <c r="P32" s="57"/>
+      <c r="Q32" s="57"/>
+      <c r="R32" s="57"/>
+      <c r="S32" s="57"/>
+      <c r="T32" s="57"/>
+      <c r="U32" s="57"/>
+      <c r="V32" s="57"/>
+      <c r="W32" s="57"/>
+      <c r="X32" s="57"/>
+      <c r="Y32" s="57"/>
+      <c r="Z32" s="57"/>
+      <c r="AA32" s="57"/>
+      <c r="AB32" s="57"/>
+      <c r="AC32" s="57"/>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A33" s="31"/>
       <c r="B33" s="31"/>
       <c r="C33" s="31"/>
@@ -11311,7 +11257,7 @@
       <c r="AB33" s="31"/>
       <c r="AC33" s="31"/>
     </row>
-    <row r="36" spans="1:29" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B36">
         <f>B23/(B23+B24)</f>
         <v>0.95262264872417801</v>
@@ -11343,7 +11289,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>179</v>
       </c>

</xml_diff>